<commit_message>
After cleaning up the data sets, including the excel file.
</commit_message>
<xml_diff>
--- a/midterm.dataset.xlsx
+++ b/midterm.dataset.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanrascon/R projects/BHDS2010/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanrascon/R projects/BHDS2010/Git Repos/Midterm.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B057C61-2001-824B-BF4D-C489A6728471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB105CC-DA72-9544-8027-3AABEC392535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{6422826E-FF9F-6548-B2DB-BF47C391E8F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t> Record </t>
   </si>
@@ -50,121 +50,10 @@
     <t>Sig.Scale </t>
   </si>
   <si>
-    <t>1 </t>
+    <t>18-35</t>
   </si>
   <si>
-    <t>18-35 </t>
-  </si>
-  <si>
-    <t>68 </t>
-  </si>
-  <si>
-    <t>7 </t>
-  </si>
-  <si>
-    <t>2 </t>
-  </si>
-  <si>
-    <t>61 </t>
-  </si>
-  <si>
-    <t>5 </t>
-  </si>
-  <si>
-    <t>3 </t>
-  </si>
-  <si>
-    <t>112 </t>
-  </si>
-  <si>
-    <t>4 </t>
-  </si>
-  <si>
-    <t>6 </t>
-  </si>
-  <si>
-    <t>111 </t>
-  </si>
-  <si>
-    <t>8 </t>
-  </si>
-  <si>
-    <t>131 </t>
-  </si>
-  <si>
-    <t>94 </t>
-  </si>
-  <si>
-    <t>59 </t>
-  </si>
-  <si>
-    <t>9 </t>
-  </si>
-  <si>
-    <t>87 </t>
-  </si>
-  <si>
-    <t>10 </t>
-  </si>
-  <si>
-    <t>96 </t>
-  </si>
-  <si>
-    <t>11 </t>
-  </si>
-  <si>
-    <t>65-80 </t>
-  </si>
-  <si>
-    <t>49 </t>
-  </si>
-  <si>
-    <t>12 </t>
-  </si>
-  <si>
-    <t>52 </t>
-  </si>
-  <si>
-    <t>13 </t>
-  </si>
-  <si>
-    <t>76 </t>
-  </si>
-  <si>
-    <t>14 </t>
-  </si>
-  <si>
-    <t>44 </t>
-  </si>
-  <si>
-    <t>15 </t>
-  </si>
-  <si>
-    <t>56 </t>
-  </si>
-  <si>
-    <t>16 </t>
-  </si>
-  <si>
-    <t>30 </t>
-  </si>
-  <si>
-    <t>17 </t>
-  </si>
-  <si>
-    <t>18 </t>
-  </si>
-  <si>
-    <t>-1 </t>
-  </si>
-  <si>
-    <t>19 </t>
-  </si>
-  <si>
-    <t>20 </t>
-  </si>
-  <si>
-    <t>25 </t>
+    <t>65-80</t>
   </si>
 </sst>
 </file>
@@ -336,13 +225,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1708CEE-C8E2-5C44-8BBE-11253AFCBD98}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1708CEE-C8E2-5C44-8BBE-11253AFCBD98}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D21" xr:uid="{F1708CEE-C8E2-5C44-8BBE-11253AFCBD98}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A3B2C60C-AD21-7B49-AAFB-EED7E60D93C7}" name=" Record " dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{AE6AACFF-EA61-154B-A77B-45C36C59FC1D}" name="Age.Group " dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D961FA9D-237B-214F-9E01-0A27CD73C0C3}" name="BSI.Total " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{14A5555D-40DB-534F-8646-7FD0F3D3AA1D}" name="Sig.Scale " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A3B2C60C-AD21-7B49-AAFB-EED7E60D93C7}" name=" Record " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{AE6AACFF-EA61-154B-A77B-45C36C59FC1D}" name="Age.Group " dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D961FA9D-237B-214F-9E01-0A27CD73C0C3}" name="BSI.Total " dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{14A5555D-40DB-534F-8646-7FD0F3D3AA1D}" name="Sig.Scale " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -665,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D88092-1982-EB47-A4E5-D81753991B37}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,284 +582,290 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>68</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>112</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>111</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>94</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>87</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>96</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>